<commit_message>
Import data from xlsx instead of json
</commit_message>
<xml_diff>
--- a/Meny hemsida.xlsx
+++ b/Meny hemsida.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_924858E5C0DEB8026F15A6DB943E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC9DA68-B1B0-42D3-A598-DE963E795CF7}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonekizean/Documents/Programmering/Brezza/brezza2.0/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{F889EA71-C739-2C4E-96D7-C384C771BDD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71645EC5-CDA9-4C19-B70B-F9D42EACD146}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>course</t>
   </si>
@@ -69,19 +74,46 @@
     <t>Buffelmozzarella med tomater, aubergine och basilika</t>
   </si>
   <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>185:-</t>
+  </si>
+  <si>
+    <t>della italia</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Secondi</t>
+  </si>
+  <si>
+    <t>Dolci</t>
+  </si>
+  <si>
+    <t>100:-</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>mmmm</t>
+  </si>
+  <si>
     <t>Avsmakning</t>
   </si>
   <si>
     <t>785:-</t>
   </si>
   <si>
-    <t>piatto piatto misto di salumi;_x000D_
-carpaccio på helleflundra;_x000D_
-ragu di coniglio;_x000D_
-osso buco;_x000D_
-sorbetto con limoncino;_x000D_
-zuppa di mare;_x000D_
-citronzabaglione;</t>
+    <t>piatto piatto misto di salumi,
+carpaccio på helleflundra,
+ragu di coniglio,
+osso buco,
+sorbetto con limoncino,
+zuppa di mare,
+citronzabaglione</t>
   </si>
   <si>
     <t>minst två personer</t>
@@ -93,17 +125,20 @@
     <t>Vinpaket</t>
   </si>
   <si>
+    <t>825:-</t>
+  </si>
+  <si>
     <t>Tre rätter</t>
   </si>
   <si>
-    <t>Vin</t>
+    <t>225:-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +150,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,12 +188,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,16 +509,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -533,52 +577,103 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="162" customHeight="1">
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="150">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="105">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="105">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate nav buttons dynamically
</commit_message>
<xml_diff>
--- a/Meny hemsida.xlsx
+++ b/Meny hemsida.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonekizean/Documents/Programmering/Brezza/brezza2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helene\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{F889EA71-C739-2C4E-96D7-C384C771BDD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71645EC5-CDA9-4C19-B70B-F9D42EACD146}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{506D7F61-EFE2-4708-A844-38403B325E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{641D4927-B752-432F-88BC-70567514FC3C}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
   <si>
     <t>course</t>
   </si>
@@ -59,10 +59,52 @@
     <t>110:-</t>
   </si>
   <si>
-    <t>Bruschetta</t>
-  </si>
-  <si>
-    <t>Citronmarinerad zicchini och tomater</t>
+    <t xml:space="preserve">Oliver &amp; parmesan med mozzarellagratinerat vitlöksbröd </t>
+  </si>
+  <si>
+    <t>Marinerade gröna oliver, parmesan och vedugnsbakat vitlöksbröd</t>
+  </si>
+  <si>
+    <t>185:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Daniele con melone </t>
+  </si>
+  <si>
+    <t>Lufttorkad skinka, sockermelon och rostade valnötter</t>
+  </si>
+  <si>
+    <t>165:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carpaccio på oxfilé </t>
+  </si>
+  <si>
+    <t>Rödvinsmarinerad oxfilé, Parmiggiano-Reggiano, citron, olivolja, tryffelemulsion, rostad mandel och ruccola</t>
+  </si>
+  <si>
+    <t>165:-/295:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piatto misto di salumi </t>
+  </si>
+  <si>
+    <t>Blandad chark, marinerade oliver, rostade hasselnötter och picklade grönsaker</t>
+  </si>
+  <si>
+    <t>145:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carpaccio på hälleflundra </t>
+  </si>
+  <si>
+    <t>Friterad grönkål, citronkräm, rostade pumpafrön och picklad morot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruschetta al forno a legna </t>
+  </si>
+  <si>
+    <t>Grillat bröd och myntamarinerade grönsaker</t>
   </si>
   <si>
     <t>135:-</t>
@@ -71,34 +113,259 @@
     <t xml:space="preserve">Mozzarella di Bufala Campana </t>
   </si>
   <si>
-    <t>Buffelmozzarella med tomater, aubergine och basilika</t>
+    <t>Buffelmozzarella med tomat, aubergine och basilika</t>
+  </si>
+  <si>
+    <t>175:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halstrade pilgrimsmusslor </t>
+  </si>
+  <si>
+    <t>Chili- och kronärtskockskräm, brynt smör och krispig Coppa di Parma</t>
   </si>
   <si>
     <t>Pasta</t>
   </si>
   <si>
-    <t>185:-</t>
-  </si>
-  <si>
-    <t>della italia</t>
+    <t>195:-</t>
+  </si>
+  <si>
+    <t>Ravioli</t>
+  </si>
+  <si>
+    <t>Spenat och ricottafylld ravioli, serveras med tomatsås och rostade pekannötter</t>
+  </si>
+  <si>
+    <t>235:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gamberi con créma di limone </t>
+  </si>
+  <si>
+    <t>Tagliatelle med stora räkor, citronsås och zucchini</t>
+  </si>
+  <si>
+    <t>225:-</t>
+  </si>
+  <si>
+    <t>Polpettini</t>
+  </si>
+  <si>
+    <t>Tagliatelle med kalvfrikadeller kokta i tomatsås</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gnocchi di casa Brezza </t>
+  </si>
+  <si>
+    <t>Gnocchi, salsicciafärs, 'nduja calabrese, soltorkade tomater och Parmigiano-Reggiano</t>
   </si>
   <si>
     <t>Pizza</t>
   </si>
   <si>
+    <t>125:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margherita </t>
+  </si>
+  <si>
+    <t>Tomatsås, mozzarella och basilika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bufalina </t>
+  </si>
+  <si>
+    <t>Buffelmozzarella, tomatsås och basilika</t>
+  </si>
+  <si>
+    <t>155:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verdure </t>
+  </si>
+  <si>
+    <t>Grillade grönsaker, tomatsås, mozzarella, lök och färsk spenat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brezza </t>
+  </si>
+  <si>
+    <t>Salsicciafärs med 'nduja calabrese, tomatsås, mozzarella, rostad paprika och oliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inferno </t>
+  </si>
+  <si>
+    <t>Salami Piccante, färsk chili, tomatsås, mozzarella, oliver, ricotta, pinjenötter och basilika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napoletana </t>
+  </si>
+  <si>
+    <t>Sardeller, kapris, tomatsås, mozzarella, oliver, oregano och basilika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frutti di Mare </t>
+  </si>
+  <si>
+    <t>Skaldjur, tomatsås, vitlöksolja, persilja, färsk spenat och citron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trentino </t>
+  </si>
+  <si>
+    <t>Prosciutto crudo från San Daniele, tomatsås, mozzarella, ruccola, soltorkade tomater och Parmigiano-Reggiano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giardino </t>
+  </si>
+  <si>
+    <t>Potatis, ägg, mozzarella, lök, soltorkade tomater, ruccola, basilikaolja och Parmigiano-Reggiano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quattro Formaggi </t>
+  </si>
+  <si>
+    <t>Gorgonzola, pecorino, mozzarella, Parmigiano-Reggiano, soltorkade tomater och pinjenötter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zola e mela </t>
+  </si>
+  <si>
+    <t>Mozzarella, gorgonzola, äpple, valnötter</t>
+  </si>
+  <si>
     <t>Secondi</t>
   </si>
   <si>
+    <t>355:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grillad oxfilé </t>
+  </si>
+  <si>
+    <t>Rostad potatis, ugnsbakade kvisttomater, ruccola, Basilikasmör och rödvinssky</t>
+  </si>
+  <si>
+    <t>275:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saltimbocca di Caza Brezza </t>
+  </si>
+  <si>
+    <t>Kalvkött med lufttorkad skinka, salviasås, ugnsbakade kvisttomater och rostad potatis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Havsaborre </t>
+  </si>
+  <si>
+    <t>Pannstekt havsabbore med ljummen färskpotatissallad och brynt smör</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grillad tonfisk </t>
+  </si>
+  <si>
+    <t>Smörslungade grönsaker och gremolata</t>
+  </si>
+  <si>
+    <t>Insalata</t>
+  </si>
+  <si>
+    <t>210:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insalata di Tonno </t>
+  </si>
+  <si>
+    <t>Grillad tonfisk, aioli, rostade pumpafrön, inlagda grönsaker, grillad citron och grönsallad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insalata salumi e formaggi </t>
+  </si>
+  <si>
+    <t>Italiensk chark &amp; ost, serveras med melon, inlagda grönsaker, olivoljevinaigrette och grönsallad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insalata misto verdure e mozzarella </t>
+  </si>
+  <si>
+    <t>Blandade färska och inlagde grönsaker, serveras med buffelmozzarella, aioli, samt rostade pecannötter och grönsallad</t>
+  </si>
+  <si>
     <t>Dolci</t>
   </si>
   <si>
-    <t>100:-</t>
-  </si>
-  <si>
-    <t>Glass</t>
-  </si>
-  <si>
-    <t>mmmm</t>
+    <t>97:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiramisu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citronzabaglione </t>
+  </si>
+  <si>
+    <t>Körsbärskompott och maräng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chokladbakelse </t>
+  </si>
+  <si>
+    <t>Dolce di latte och jordgubbssorbet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pannacotta di lampone </t>
+  </si>
+  <si>
+    <t>Hallonpannacotta med pistagesmulor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorbeto di fragola con spumante </t>
+  </si>
+  <si>
+    <t>Jordgubbssorbet toppad med spumante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorbetto con limoncino </t>
+  </si>
+  <si>
+    <t>Blodapelsinsorbet toppad med Limoncino</t>
+  </si>
+  <si>
+    <t>45:-/75:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gelato/Sorbet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Välj mellan fyra hemgjorda glassar; Vaniljglass, valnötsglass, jordgubbssorbet eller blodapelsinsorbet </t>
+  </si>
+  <si>
+    <t>45:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chokladtryffel </t>
+  </si>
+  <si>
+    <t>Välj mellan lakrits eller naturell</t>
+  </si>
+  <si>
+    <t>95:-/125:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piatto misto di formaggi </t>
+  </si>
+  <si>
+    <t>Två eller tre ostar, serveras med hemgjord marmelad</t>
+  </si>
+  <si>
+    <t>115:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantucci con Vinsanto </t>
+  </si>
+  <si>
+    <t>Hemgjord mandelkaka, serveras med dessertvin från Toscana</t>
   </si>
   <si>
     <t>Avsmakning</t>
@@ -107,13 +374,13 @@
     <t>785:-</t>
   </si>
   <si>
-    <t>piatto piatto misto di salumi,
-carpaccio på helleflundra,
-ragu di coniglio,
-osso buco,
-sorbetto con limoncino,
-zuppa di mare,
-citronzabaglione</t>
+    <t>san daniele con melone,
+carpaccio på hälleflundra, 
+ravioli, 
+grillad oxfilé, 
+sorbetto,
+havsabborre, 
+pannacotta di lampone</t>
   </si>
   <si>
     <t>minst två personer</t>
@@ -128,10 +395,17 @@
     <t>825:-</t>
   </si>
   <si>
+    <t>539:-</t>
+  </si>
+  <si>
+    <t>Halstrade pilgrimsmusslor, 
+Saltimbocca di Casa Brezza eller Grillad tonfisk, Chokladbakelse</t>
+  </si>
+  <si>
     <t>Tre rätter</t>
   </si>
   <si>
-    <t>225:-</t>
+    <t>395:-</t>
   </si>
 </sst>
 </file>
@@ -188,13 +462,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,18 +784,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" customWidth="1"/>
+    <col min="4" max="4" width="62" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
@@ -556,7 +831,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
@@ -579,13 +854,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -593,90 +868,564 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="105">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="105">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s">
-        <v>31</v>
+      <c r="C31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="117" customHeight="1">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="84.75" customHeight="1">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G43" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>